<commit_message>
New fixes to GHG processing templates
</commit_message>
<xml_diff>
--- a/Synoptic/Template_GHG_GCHeadspace.xlsx
+++ b/Synoptic/Template_GHG_GCHeadspace.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carla López Lloreda\Dropbox\Grad school\Research\Delmarva project\Data\Synoptic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA29B527-6A24-4E0B-9375-04C4144F3F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A40177-FCFB-4AB8-B9C2-7F50B7EDFD01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B9F46523-41A8-448F-A46A-C2D7363E9E8A}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>GC_Number</t>
   </si>
@@ -105,12 +105,6 @@
     <t>GC_ID</t>
   </si>
   <si>
-    <t>Water_Temp_DegC</t>
-  </si>
-  <si>
-    <t>Ambient_air</t>
-  </si>
-  <si>
     <t>Precision</t>
   </si>
   <si>
@@ -127,13 +121,22 @@
   </si>
   <si>
     <t>WaterV_mL</t>
+  </si>
+  <si>
+    <t>Air_Location</t>
+  </si>
+  <si>
+    <t>Has been changed thru samplings</t>
+  </si>
+  <si>
+    <t>WaterT_C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,12 +151,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -514,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEEB0679-200B-40E0-8249-72636D6E4DAF}">
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -530,7 +527,7 @@
     <col min="7" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.44140625" customWidth="1"/>
     <col min="13" max="13" width="13.109375" customWidth="1"/>
-    <col min="15" max="15" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="28.21875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15" customWidth="1"/>
     <col min="22" max="22" width="10.88671875" customWidth="1"/>
   </cols>
@@ -579,27 +576,35 @@
         <v>13</v>
       </c>
       <c r="O1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="R1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="U1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="V1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="O2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added columns for air averages to template
</commit_message>
<xml_diff>
--- a/Synoptic/Template_GHG_GCHeadspace.xlsx
+++ b/Synoptic/Template_GHG_GCHeadspace.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carla López Lloreda\Dropbox\Grad school\Research\Delmarva project\Data\Synoptic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carla López Lloreda\Dropbox\Grad school\Research\Delmarva project\Projects\Synoptic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A40177-FCFB-4AB8-B9C2-7F50B7EDFD01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62CB0E3-A7F7-4C35-9E27-D532AF6E2130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B9F46523-41A8-448F-A46A-C2D7363E9E8A}"/>
   </bookViews>
@@ -48,7 +48,7 @@
     This comes from analytical lab data</t>
       </text>
     </comment>
-    <comment ref="I1" authorId="1" shapeId="0" xr:uid="{DA4C92BE-39B9-4219-B158-23C8539F0ECA}">
+    <comment ref="K1" authorId="1" shapeId="0" xr:uid="{DA4C92BE-39B9-4219-B158-23C8539F0ECA}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>GC_Number</t>
   </si>
@@ -130,6 +130,33 @@
   </si>
   <si>
     <t>WaterT_C</t>
+  </si>
+  <si>
+    <t>Site</t>
+  </si>
+  <si>
+    <t>Sample_Type</t>
+  </si>
+  <si>
+    <t>Need to add in old samplings</t>
+  </si>
+  <si>
+    <t>AirCO2_med_ppm</t>
+  </si>
+  <si>
+    <t>AirCO2_min_ppm</t>
+  </si>
+  <si>
+    <t>AirCO2_max_ppm</t>
+  </si>
+  <si>
+    <t>AirCH4_med_ppm</t>
+  </si>
+  <si>
+    <t>AirCH4_min_ppm</t>
+  </si>
+  <si>
+    <t>AirCH4_max_ppm</t>
   </si>
 </sst>
 </file>
@@ -503,7 +530,7 @@
   <threadedComment ref="A1" dT="2021-10-05T21:58:29.81" personId="{27529C29-9444-4767-A99F-FB63B97BEEA9}" id="{803444A8-F390-4B7A-AEC7-1393D3711324}">
     <text>This comes from analytical lab data</text>
   </threadedComment>
-  <threadedComment ref="I1" dT="2021-10-05T21:59:05.94" personId="{27529C29-9444-4767-A99F-FB63B97BEEA9}" id="{DA4C92BE-39B9-4219-B158-23C8539F0ECA}">
+  <threadedComment ref="K1" dT="2021-10-05T21:59:05.94" personId="{27529C29-9444-4767-A99F-FB63B97BEEA9}" id="{DA4C92BE-39B9-4219-B158-23C8539F0ECA}">
     <text>This comes from field data (Key)</text>
   </threadedComment>
 </ThreadedComments>
@@ -511,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEEB0679-200B-40E0-8249-72636D6E4DAF}">
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -525,14 +552,16 @@
     <col min="4" max="5" width="9.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.44140625" customWidth="1"/>
-    <col min="13" max="13" width="13.109375" customWidth="1"/>
-    <col min="15" max="15" width="28.21875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15" customWidth="1"/>
-    <col min="22" max="22" width="10.88671875" customWidth="1"/>
+    <col min="9" max="9" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.44140625" customWidth="1"/>
+    <col min="15" max="15" width="13.109375" customWidth="1"/>
+    <col min="17" max="17" width="28.21875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15" customWidth="1"/>
+    <col min="24" max="24" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -558,53 +587,83 @@
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="Y1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O2" t="s">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="I2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" t="s">
         <v>21</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removing area and retention time columns from template spreadsheet
</commit_message>
<xml_diff>
--- a/Synoptic/Template_GHG_GCHeadspace.xlsx
+++ b/Synoptic/Template_GHG_GCHeadspace.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carla López Lloreda\Dropbox\Grad school\Research\Delmarva project\Projects\Synoptic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62CB0E3-A7F7-4C35-9E27-D532AF6E2130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE14018-1476-4B14-B993-39F2B13973FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B9F46523-41A8-448F-A46A-C2D7363E9E8A}"/>
   </bookViews>
@@ -48,7 +48,7 @@
     This comes from analytical lab data</t>
       </text>
     </comment>
-    <comment ref="K1" authorId="1" shapeId="0" xr:uid="{DA4C92BE-39B9-4219-B158-23C8539F0ECA}">
+    <comment ref="G1" authorId="1" shapeId="0" xr:uid="{DA4C92BE-39B9-4219-B158-23C8539F0ECA}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>GC_Number</t>
   </si>
@@ -69,19 +69,7 @@
     <t>GC_SampleID</t>
   </si>
   <si>
-    <t>CH4_RetTime</t>
-  </si>
-  <si>
-    <t>CH4_Area</t>
-  </si>
-  <si>
     <t>CH4_ppm</t>
-  </si>
-  <si>
-    <t>CO2_RetTime</t>
-  </si>
-  <si>
-    <t>CO2_Area</t>
   </si>
   <si>
     <t>CO2_ppm</t>
@@ -530,7 +518,7 @@
   <threadedComment ref="A1" dT="2021-10-05T21:58:29.81" personId="{27529C29-9444-4767-A99F-FB63B97BEEA9}" id="{803444A8-F390-4B7A-AEC7-1393D3711324}">
     <text>This comes from analytical lab data</text>
   </threadedComment>
-  <threadedComment ref="K1" dT="2021-10-05T21:59:05.94" personId="{27529C29-9444-4767-A99F-FB63B97BEEA9}" id="{DA4C92BE-39B9-4219-B158-23C8539F0ECA}">
+  <threadedComment ref="G1" dT="2021-10-05T21:59:05.94" personId="{27529C29-9444-4767-A99F-FB63B97BEEA9}" id="{DA4C92BE-39B9-4219-B158-23C8539F0ECA}">
     <text>This comes from field data (Key)</text>
   </threadedComment>
 </ThreadedComments>
@@ -538,30 +526,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEEB0679-200B-40E0-8249-72636D6E4DAF}">
-  <dimension ref="A1:AD2"/>
+  <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.109375" customWidth="1"/>
     <col min="2" max="2" width="14.109375" customWidth="1"/>
-    <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.44140625" customWidth="1"/>
-    <col min="15" max="15" width="13.109375" customWidth="1"/>
-    <col min="17" max="17" width="28.21875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15" customWidth="1"/>
-    <col min="24" max="24" width="10.88671875" customWidth="1"/>
+    <col min="3" max="3" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.44140625" customWidth="1"/>
+    <col min="11" max="11" width="13.109375" customWidth="1"/>
+    <col min="13" max="13" width="28.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15" customWidth="1"/>
+    <col min="20" max="20" width="10.88671875" customWidth="1"/>
+    <col min="21" max="21" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -575,64 +561,64 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="S1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>17</v>
+      <c r="V1" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>26</v>
@@ -640,31 +626,19 @@
       <c r="Z1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AA1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>31</v>
-      </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="I2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q2" t="s">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
         <v>21</v>
       </c>
-      <c r="R2" t="s">
+      <c r="F2" t="s">
         <v>21</v>
+      </c>
+      <c r="M2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>